<commit_message>
Atualizando excel e adicionando o relatorio em pdf/word
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade\Ciência da Computação - FEI\8º Semestre\Segurança\at02\SegurancaHash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C127A475-B96B-43F4-BD37-E79F2C1AC15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15A940F-0D0F-4AE5-A2DD-575CC4070722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DFBCA40-2FEB-4A22-A0C6-24D51441A517}"/>
   </bookViews>
@@ -192,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +210,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,16 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,6 +281,12 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,17 +604,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB596C87-CCB0-4E54-98E4-01113397EE9B}">
   <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.5546875" customWidth="1"/>
-    <col min="4" max="4" width="52.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" style="5" customWidth="1"/>
     <col min="5" max="5" width="36.88671875" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" style="5" customWidth="1"/>
     <col min="7" max="7" width="28.109375" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" customWidth="1"/>
   </cols>
@@ -639,19 +649,19 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -662,19 +672,19 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -685,19 +695,19 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -708,19 +718,19 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -731,19 +741,19 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -754,19 +764,19 @@
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -777,19 +787,19 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -800,19 +810,19 @@
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -823,19 +833,19 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -846,24 +856,24 @@
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="7"/>
+      <c r="D13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>